<commit_message>
Added a new function numeric_data_frame to convert all columns of a data frame to numeric, with a nice error message about the texts that could not be converted.
</commit_message>
<xml_diff>
--- a/examples/read_ts/xlsx/example1.xlsx
+++ b/examples/read_ts/xlsx/example1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="996" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="example1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t xml:space="preserve">Output of the CEP 2017</t>
   </si>
@@ -53,6 +53,12 @@
   </si>
   <si>
     <t xml:space="preserve">2011Q1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">klaas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jan</t>
   </si>
   <si>
     <t xml:space="preserve">2011Q2</t>
@@ -161,19 +167,19 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.8877551020408"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.3061224489796"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.3571428571429"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2142857142857"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.3571428571429"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.2142857142857"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.1632653061224"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="12.2142857142857"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.8265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.8775510204082"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -228,8 +234,11 @@
       <c r="B7" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="0" t="n">
-        <v>5</v>
+      <c r="C7" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>12</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>50</v>
@@ -237,7 +246,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>6</v>
@@ -248,10 +257,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>